<commit_message>
added more for write music
</commit_message>
<xml_diff>
--- a/optical_filter_set.xlsx
+++ b/optical_filter_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cneveu\Documents\GitHub\VSD_CFE_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50721D97-0CB9-4F49-84A6-7A3CE22A9FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79E4840-74F3-4C37-8D8D-5ECB6D09BFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="di-4-ANNEPS" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Excitation</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>Emmision</t>
   </si>
 </sst>
 </file>
@@ -256,6 +259,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>493714</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>132857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32D3C23D-6D71-44CB-9ED8-289DF4D23EB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3800475" y="10877550"/>
+          <a:ext cx="12685714" cy="3942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -522,13 +569,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -603,6 +653,27 @@
       </c>
       <c r="P12" s="5" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>605</v>
+      </c>
+      <c r="C14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on ROI warp,
 its not moving ROIs in whole recording
</commit_message>
<xml_diff>
--- a/optical_filter_set.xlsx
+++ b/optical_filter_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cneveu\Documents\GitHub\VSD_CFE_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4CFC0B-2422-43DC-93C6-3A9CBACD920F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D435E7-A0B7-44E2-9284-D273360ECDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32070" yWindow="1480" windowWidth="29040" windowHeight="14390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-33750" yWindow="3510" windowWidth="28800" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="di-4-ANNEPS" sheetId="1" r:id="rId1"/>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +932,7 @@
   <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
recent menu now working
</commit_message>
<xml_diff>
--- a/optical_filter_set.xlsx
+++ b/optical_filter_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cneveu\Documents\GitHub\VSD_CFE_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CCD1B1-97BD-44A2-8B58-70AB3C57BA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BD52AE-1A77-4015-8409-A067D965D0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37910" yWindow="430" windowWidth="26070" windowHeight="18290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37240" yWindow="1420" windowWidth="28800" windowHeight="15450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="di-4-ANNEPS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Excitation</t>
   </si>
@@ -165,6 +165,33 @@
   </si>
   <si>
     <t>https://www.researchgate.net/publication/374262345_Recent_advances_and_current_limitations_of_available_technology_to_optically_manipulate_and_observe_cardiac_electrophysiology</t>
+  </si>
+  <si>
+    <t>Dichroic mirror</t>
+  </si>
+  <si>
+    <t>Emission Filter</t>
+  </si>
+  <si>
+    <t>Filter Cube</t>
+  </si>
+  <si>
+    <t>Parts</t>
+  </si>
+  <si>
+    <t>Dyes</t>
+  </si>
+  <si>
+    <t>X-Rhod-1</t>
+  </si>
+  <si>
+    <t>Cal-630</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -229,12 +256,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -243,13 +285,20 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -976,13 +1025,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868D9A46-42E3-4EDC-8147-D1FB147932EC}">
-  <dimension ref="A4:D22"/>
+  <dimension ref="A4:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1014,12 +1068,94 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
       <c r="B22" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" s="8">
+        <v>250</v>
+      </c>
+      <c r="J29" s="8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I30" s="8">
+        <v>365</v>
+      </c>
+      <c r="J30" s="8">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H31" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="8">
+        <v>494</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H32" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H33" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="8">
+        <v>454</v>
+      </c>
+      <c r="J33" s="8">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H34" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I34" s="8">
+        <v>341</v>
+      </c>
+      <c r="J34" s="8">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H35" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="10">
+        <f>SUM(I29:I34)</f>
+        <v>1904</v>
+      </c>
+      <c r="J35" s="10">
+        <f>SUM(J29:J34)</f>
+        <v>1410</v>
       </c>
     </row>
   </sheetData>
@@ -1029,6 +1165,7 @@
     <hyperlink ref="D5" r:id="rId3" xr:uid="{524C7927-67A3-47B2-AC64-D6F597788B8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>